<commit_message>
sistemazione file excel, json e inserimento dati nel database
</commit_message>
<xml_diff>
--- a/Java/BGTransport/src/main/resources/excel/companies_list.xlsx
+++ b/Java/BGTransport/src/main/resources/excel/companies_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/86d5980519d90a03/Desktop/BGTransports/Java/BGTransport/src/main/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{55FF970F-97E2-48B1-882E-D374F3833327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D42BA21-EF84-437D-9261-F7781A7C6A9D}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{55FF970F-97E2-48B1-882E-D374F3833327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B93A58D9-7473-4FE6-A7A3-3BDCEAE239DD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D46561FF-82E1-4E07-BAED-B02E6297CA5D}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
-    <t>CAP</t>
-  </si>
-  <si>
     <t>ATB SERVIZI</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>legal_structure</t>
   </si>
   <si>
-    <t>ATECO_code</t>
-  </si>
-  <si>
     <t>business_tax_code</t>
   </si>
   <si>
@@ -220,13 +214,19 @@
   </si>
   <si>
     <t>02605730163</t>
+  </si>
+  <si>
+    <t>ateco_code</t>
+  </si>
+  <si>
+    <t>cap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,13 +261,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -290,12 +283,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -711,10 +703,10 @@
     <tableColumn id="5" xr3:uid="{C91AAAE7-D435-4838-9419-C64DB88D2873}" name="incorporation_date" dataDxfId="12"/>
     <tableColumn id="6" xr3:uid="{1083CA1F-440F-41D2-8EFC-739B4201C880}" name="legal_representative" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{F5E3F39F-5D3D-4111-83E5-33F8CE2C2498}" name="number_of_employees" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{E323C77A-F5F3-4DC6-8CE1-3E45B8A4346A}" name="ATECO_code" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{E323C77A-F5F3-4DC6-8CE1-3E45B8A4346A}" name="ateco_code" dataDxfId="9"/>
     <tableColumn id="9" xr3:uid="{7259A6A0-D349-462E-A41F-9D156EFA6202}" name="registered_office" dataDxfId="8"/>
     <tableColumn id="10" xr3:uid="{35302CA6-6D1E-4AA7-8A3B-716E6BD73B3F}" name="province" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{1EAB0CDF-5AEB-4E29-91C2-2925663C5371}" name="CAP" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{1EAB0CDF-5AEB-4E29-91C2-2925663C5371}" name="cap" dataDxfId="6"/>
     <tableColumn id="12" xr3:uid="{276C87D7-1D1D-4834-8A3C-1DA860D745BD}" name="address" dataDxfId="5"/>
     <tableColumn id="13" xr3:uid="{5262E237-9767-424A-A802-D2B330E70FD3}" name="street_number" dataDxfId="4"/>
     <tableColumn id="14" xr3:uid="{DA593B5B-7936-4979-8E3A-470DCB59C8F5}" name="telephone" dataDxfId="3"/>
@@ -1046,7 +1038,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,263 +1064,263 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2003</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2003</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="2">
+        <v>332</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4931</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3">
-        <v>332</v>
-      </c>
-      <c r="H2" s="3">
-        <v>4931</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="2">
+        <v>24125</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3">
-        <v>24125</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="2">
+        <v>13</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="3">
-        <v>13</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2002</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <v>1510</v>
+      </c>
+      <c r="H3" s="2">
+        <v>493</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="3">
-        <v>2002</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3">
-        <v>1510</v>
-      </c>
-      <c r="H3" s="3">
-        <v>493</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="2">
+        <v>20132</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="3">
-        <v>20132</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="2">
+        <v>11</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="3">
-        <v>11</v>
-      </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1998</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="2">
+        <v>126</v>
+      </c>
+      <c r="H4" s="2">
+        <v>4931</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="2">
+        <v>24126</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="3">
-        <v>126</v>
-      </c>
-      <c r="H4" s="3">
-        <v>4931</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="3">
-        <v>24126</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="2">
+        <v>17</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="3">
-        <v>17</v>
-      </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2011</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
+        <v>4708</v>
+      </c>
+      <c r="H5" s="2">
+        <v>491</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="J5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="2">
+        <v>20123</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2011</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3">
-        <v>4708</v>
-      </c>
-      <c r="H5" s="3">
-        <v>491</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="M5" s="2">
         <v>14</v>
       </c>
-      <c r="K5" s="3">
-        <v>20123</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="3">
-        <v>14</v>
-      </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>